<commit_message>
added some analysis to chicken_wings
</commit_message>
<xml_diff>
--- a/chicken_wings/data/Chicken_Wings.xlsx
+++ b/chicken_wings/data/Chicken_Wings.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/Documents/code/chicken_wings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ABABD8-01AC-8D48-90C0-8D21511FC25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46BDDAD-57FE-EA47-95CB-D041BD81D4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{29090A6C-1064-F541-B044-7FA7E10DFA86}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="34200" windowHeight="21400" activeTab="1" xr2:uid="{29090A6C-1064-F541-B044-7FA7E10DFA86}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Graphs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,26 +121,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -161,74 +151,10 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -250,12 +176,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -269,19 +189,1288 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Cost of Wing (cents / wing)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Main!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg Wing Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Main!$A$3:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Main!$C$3:$C$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>113.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>113.33333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>113.57143000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113.33333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>113.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>113.63636</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>113.33333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>113.46154</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>113.57143000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>113.33333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>113.4375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>113.52941</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>113.33333</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>113.42104999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>113.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>113.33333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>113.40909000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>113.47826000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>113.54167</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>111.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>111.34614999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>111.48148</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>111.42856999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>111.55172</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>111.66667</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>111.85714</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>112.22221999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>111.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>111.66667</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>111.85714</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>111.26667</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>111.375</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>111.61111</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>111.25</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>111.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>111.23333</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>111.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D23A-304B-9232-9B9D4737A0FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1141537759"/>
+        <c:axId val="1412501887"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1141537759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Quantity of Chicken Wings</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1412501887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1412501887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Cost of One Wing (cents)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1141537759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19449</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>24255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>91530</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171621</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A439E2A1-3EE2-BF2D-8160-9EFD347304EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A87C0F6-9030-B44A-BC2D-5A0DC443417F}" name="Chicken_Wings" displayName="Chicken_Wings" ref="A2:F42" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A87C0F6-9030-B44A-BC2D-5A0DC443417F}" name="Chicken_Wings" displayName="Chicken_Wings" ref="A2:F42" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A2:F42" xr:uid="{6A87C0F6-9030-B44A-BC2D-5A0DC443417F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{360FF5DA-433B-A846-80A8-BB55B2FD853B}" name="Quantity"/>
-    <tableColumn id="2" xr3:uid="{E15EF650-6850-DA48-B759-176066E221B9}" name="Cost" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B773AF77-6649-9C4F-9477-00A6AE7338D0}" name="Avg Wing Cost" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{E15EF650-6850-DA48-B759-176066E221B9}" name="Cost" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{B773AF77-6649-9C4F-9477-00A6AE7338D0}" name="Avg Wing Cost" dataDxfId="3">
       <calculatedColumnFormula>ROUND(B3/A3,5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{99880E7A-D9F5-514D-BDA0-E87C296F30C7}" name="Change in Wing Amount">
       <calculatedColumnFormula>A3-A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{49E17064-3D36-8442-83E6-414BD323AEB6}" name="Increase in Cost" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{49E17064-3D36-8442-83E6-414BD323AEB6}" name="Increase in Cost" dataDxfId="2">
       <calculatedColumnFormula>B3-B2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{F17287B4-B1BC-D147-8F8D-24C330546FFC}" name="Avg Cost Increase">
@@ -611,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614A498D-8EB1-0644-9825-C15506081E5F}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,22 +1835,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -669,960 +1858,960 @@
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>4.55</v>
+      <c r="B3">
+        <v>455</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C42" si="0">ROUND(B3/A3,5)</f>
-        <v>1.1375</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+        <v>113.75</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
-        <v>5.7</v>
+      <c r="B4">
+        <v>570</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>1.1399999999999999</v>
+        <v>114</v>
       </c>
       <c r="D4">
         <f>A4-A3</f>
         <v>1</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <f>B4-B3</f>
-        <v>1.1500000000000004</v>
+        <v>115</v>
       </c>
       <c r="F4">
         <f>E4/D4</f>
-        <v>1.1500000000000004</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
-        <v>6.8</v>
+      <c r="B5">
+        <v>680</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>1.1333299999999999</v>
+        <v>113.33333</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D42" si="1">A5-A4</f>
         <v>1</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
         <f t="shared" ref="E5:E42" si="2">B5-B4</f>
-        <v>1.0999999999999996</v>
+        <v>110</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F42" si="3">E5/D5</f>
-        <v>1.0999999999999996</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
-        <v>7.95</v>
+      <c r="B6">
+        <v>795</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>1.13571</v>
+        <v>113.57143000000001</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000004</v>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>1.1500000000000004</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
-        <v>9.1</v>
+      <c r="B7">
+        <v>910</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1.1375</v>
+        <v>113.75</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999995</v>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>1.1499999999999995</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
-        <v>10.199999999999999</v>
+      <c r="B8">
+        <v>1019.9999999999999</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1.1333299999999999</v>
+        <v>113.33333</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E8" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0999999999999996</v>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>109.99999999999989</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>1.0999999999999996</v>
+        <v>109.99999999999989</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
-        <v>11.35</v>
+      <c r="B9">
+        <v>1135</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.135</v>
+        <v>113.5</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000004</v>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>115.00000000000011</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>1.1500000000000004</v>
+        <v>115.00000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
-        <v>12.5</v>
+      <c r="B10">
+        <v>1250</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1.13636</v>
+        <v>113.63636</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E10" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000004</v>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>1.1500000000000004</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
-        <v>13.6</v>
+      <c r="B11">
+        <v>1360</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>1.1333299999999999</v>
+        <v>113.33333</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0999999999999996</v>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>1.0999999999999996</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
-        <v>14.75</v>
+      <c r="B12">
+        <v>1475</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>1.13462</v>
+        <v>113.46154</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000004</v>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>1.1500000000000004</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>14</v>
       </c>
-      <c r="B13" s="1">
-        <v>15.9</v>
+      <c r="B13">
+        <v>1590</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>1.13571</v>
+        <v>113.57143000000001</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E13" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000004</v>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>1.1500000000000004</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>15</v>
       </c>
-      <c r="B14" s="1">
-        <v>17</v>
+      <c r="B14">
+        <v>1700</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>1.1333299999999999</v>
+        <v>113.33333</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E14" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0999999999999996</v>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>1.0999999999999996</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>16</v>
       </c>
-      <c r="B15" s="1">
-        <v>18.149999999999999</v>
+      <c r="B15">
+        <v>1814.9999999999998</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>1.1343799999999999</v>
+        <v>113.4375</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E15" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999986</v>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>114.99999999999977</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>1.1499999999999986</v>
+        <v>114.99999999999977</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>17</v>
       </c>
-      <c r="B16" s="1">
-        <v>19.3</v>
+      <c r="B16">
+        <v>1930</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>1.1352899999999999</v>
+        <v>113.52941</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E16" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000021</v>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>115.00000000000023</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>1.1500000000000021</v>
+        <v>115.00000000000023</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>18</v>
       </c>
-      <c r="B17" s="1">
-        <v>20.399999999999999</v>
+      <c r="B17">
+        <v>2039.9999999999998</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>1.1333299999999999</v>
+        <v>113.33333</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E17" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0999999999999979</v>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>109.99999999999977</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>1.0999999999999979</v>
+        <v>109.99999999999977</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>19</v>
       </c>
-      <c r="B18" s="1">
-        <v>21.55</v>
+      <c r="B18">
+        <v>2155</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>1.1342099999999999</v>
+        <v>113.42104999999999</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E18" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000021</v>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>115.00000000000023</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>1.1500000000000021</v>
+        <v>115.00000000000023</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20</v>
       </c>
-      <c r="B19" s="1">
-        <v>22.7</v>
+      <c r="B19">
+        <v>2270</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1.135</v>
+        <v>113.5</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E19" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999986</v>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
-        <v>1.1499999999999986</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>21</v>
       </c>
-      <c r="B20" s="1">
-        <v>23.8</v>
+      <c r="B20">
+        <v>2380</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>1.1333299999999999</v>
+        <v>113.33333</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E20" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1000000000000014</v>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>1.1000000000000014</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>22</v>
       </c>
-      <c r="B21" s="1">
-        <v>24.95</v>
+      <c r="B21">
+        <v>2495</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>1.13409</v>
+        <v>113.40909000000001</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E21" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999986</v>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>1.1499999999999986</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>23</v>
       </c>
-      <c r="B22" s="1">
-        <v>26.1</v>
+      <c r="B22">
+        <v>2610</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>1.1347799999999999</v>
+        <v>113.47826000000001</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E22" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000021</v>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F22">
         <f t="shared" si="3"/>
-        <v>1.1500000000000021</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>24</v>
       </c>
-      <c r="B23" s="1">
-        <v>27.25</v>
+      <c r="B23">
+        <v>2725</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>1.1354200000000001</v>
+        <v>113.54167</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E23" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999986</v>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>1.1499999999999986</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>25</v>
       </c>
-      <c r="B24" s="1">
-        <v>27.8</v>
+      <c r="B24">
+        <v>2780</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>1.1120000000000001</v>
+        <v>111.2</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E24" s="1">
-        <f t="shared" si="2"/>
-        <v>0.55000000000000071</v>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>55</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
-        <v>0.55000000000000071</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>26</v>
       </c>
-      <c r="B25" s="1">
-        <v>28.95</v>
+      <c r="B25">
+        <v>2895</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>1.1134599999999999</v>
+        <v>111.34614999999999</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E25" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999986</v>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>1.1499999999999986</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>27</v>
       </c>
-      <c r="B26" s="1">
-        <v>30.1</v>
+      <c r="B26">
+        <v>3010</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>1.1148100000000001</v>
+        <v>111.48148</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E26" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000021</v>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>1.1500000000000021</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>28</v>
       </c>
-      <c r="B27" s="1">
-        <v>31.2</v>
+      <c r="B27">
+        <v>3120</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>1.11429</v>
+        <v>111.42856999999999</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E27" s="1">
-        <f t="shared" si="2"/>
-        <v>1.0999999999999979</v>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>110</v>
       </c>
       <c r="F27">
         <f t="shared" si="3"/>
-        <v>1.0999999999999979</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>29</v>
       </c>
-      <c r="B28" s="1">
-        <v>32.35</v>
+      <c r="B28">
+        <v>3235</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>1.1155200000000001</v>
+        <v>111.55172</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E28" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1500000000000021</v>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F28">
         <f t="shared" si="3"/>
-        <v>1.1500000000000021</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>30</v>
       </c>
-      <c r="B29" s="1">
-        <v>33.5</v>
+      <c r="B29">
+        <v>3350</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>1.1166700000000001</v>
+        <v>111.66667</v>
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E29" s="1">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999986</v>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="F29">
         <f t="shared" si="3"/>
-        <v>1.1499999999999986</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>35</v>
       </c>
-      <c r="B30" s="1">
-        <v>39.15</v>
+      <c r="B30">
+        <v>3915</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>1.1185700000000001</v>
+        <v>111.85714</v>
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E30" s="1">
-        <f t="shared" si="2"/>
-        <v>5.6499999999999986</v>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>565</v>
       </c>
       <c r="F30">
         <f t="shared" si="3"/>
-        <v>1.1299999999999997</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>40</v>
       </c>
-      <c r="B31" s="1">
-        <v>44.8</v>
+      <c r="B31">
+        <v>4480</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>112</v>
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E31" s="1">
-        <f t="shared" si="2"/>
-        <v>5.6499999999999986</v>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>565</v>
       </c>
       <c r="F31">
         <f t="shared" si="3"/>
-        <v>1.1299999999999997</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>45</v>
       </c>
-      <c r="B32" s="1">
-        <v>50.5</v>
+      <c r="B32">
+        <v>5050</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>1.12222</v>
+        <v>112.22221999999999</v>
       </c>
       <c r="D32">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E32" s="1">
-        <f t="shared" si="2"/>
-        <v>5.7000000000000028</v>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>570</v>
       </c>
       <c r="F32">
         <f t="shared" si="3"/>
-        <v>1.1400000000000006</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>50</v>
       </c>
-      <c r="B33" s="1">
-        <v>55.6</v>
+      <c r="B33">
+        <v>5560</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>1.1120000000000001</v>
+        <v>111.2</v>
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E33" s="1">
-        <f t="shared" si="2"/>
-        <v>5.1000000000000014</v>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>510</v>
       </c>
       <c r="F33">
         <f t="shared" si="3"/>
-        <v>1.0200000000000002</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>60</v>
       </c>
-      <c r="B34" s="1">
-        <v>67</v>
+      <c r="B34">
+        <v>6700</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>1.1166700000000001</v>
+        <v>111.66667</v>
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E34" s="1">
-        <f t="shared" si="2"/>
-        <v>11.399999999999999</v>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>1140</v>
       </c>
       <c r="F34">
         <f t="shared" si="3"/>
-        <v>1.1399999999999999</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>70</v>
       </c>
-      <c r="B35" s="1">
-        <v>78.3</v>
+      <c r="B35">
+        <v>7830</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>1.1185700000000001</v>
+        <v>111.85714</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E35" s="1">
-        <f t="shared" si="2"/>
-        <v>11.299999999999997</v>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>1130</v>
       </c>
       <c r="F35">
         <f t="shared" si="3"/>
-        <v>1.1299999999999997</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>75</v>
       </c>
-      <c r="B36" s="1">
-        <v>83.45</v>
+      <c r="B36">
+        <v>8345</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>1.11267</v>
+        <v>111.26667</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E36" s="1">
-        <f t="shared" si="2"/>
-        <v>5.1500000000000057</v>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>515</v>
       </c>
       <c r="F36">
         <f t="shared" si="3"/>
-        <v>1.0300000000000011</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>80</v>
       </c>
-      <c r="B37" s="1">
-        <v>89.1</v>
+      <c r="B37">
+        <v>8910</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>1.11375</v>
+        <v>111.375</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="E37" s="1">
-        <f t="shared" si="2"/>
-        <v>5.6499999999999915</v>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>565</v>
       </c>
       <c r="F37">
         <f t="shared" si="3"/>
-        <v>1.1299999999999983</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>90</v>
       </c>
-      <c r="B38" s="1">
-        <v>100.45</v>
+      <c r="B38">
+        <v>10045</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>1.1161099999999999</v>
+        <v>111.61111</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E38" s="1">
-        <f t="shared" si="2"/>
-        <v>11.350000000000009</v>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>1135</v>
       </c>
       <c r="F38">
         <f t="shared" si="3"/>
-        <v>1.1350000000000009</v>
+        <v>113.5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>100</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
+        <v>11125</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
         <v>111.25</v>
       </c>
-      <c r="C39">
-        <f t="shared" si="0"/>
-        <v>1.1125</v>
-      </c>
       <c r="D39">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="E39" s="1">
-        <f t="shared" si="2"/>
-        <v>10.799999999999997</v>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>1080</v>
       </c>
       <c r="F39">
         <f t="shared" si="3"/>
-        <v>1.0799999999999996</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>125</v>
       </c>
-      <c r="B40" s="1">
-        <v>139</v>
+      <c r="B40">
+        <v>13900</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>1.1120000000000001</v>
+        <v>111.2</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="E40" s="1">
-        <f t="shared" si="2"/>
-        <v>27.75</v>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>2775</v>
       </c>
       <c r="F40">
         <f t="shared" si="3"/>
-        <v>1.1100000000000001</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>150</v>
       </c>
-      <c r="B41" s="1">
-        <v>166.85</v>
+      <c r="B41">
+        <v>16685</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>1.11233</v>
+        <v>111.23333</v>
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="E41" s="1">
-        <f t="shared" si="2"/>
-        <v>27.849999999999994</v>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>2785</v>
       </c>
       <c r="F41">
         <f t="shared" si="3"/>
-        <v>1.1139999999999999</v>
+        <v>111.4</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>200</v>
       </c>
-      <c r="B42" s="1">
-        <v>222.5</v>
+      <c r="B42">
+        <v>22250</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>1.1125</v>
+        <v>111.25</v>
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="E42" s="1">
-        <f t="shared" si="2"/>
-        <v>55.650000000000006</v>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>5565</v>
       </c>
       <c r="F42">
         <f t="shared" si="3"/>
-        <v>1.1130000000000002</v>
+        <v>111.3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C42">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>C3=MAX($C$3:$C$42)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>C3=MIN($C$3:$C$42)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>C3=MAX($C$3:$C$42)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1630,4 +2819,19 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60157A21-0BBD-8349-8176-E3F8EFEA4634}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
set up environment files and worked on retail dataset
</commit_message>
<xml_diff>
--- a/chicken_wings/data/Chicken_Wings.xlsx
+++ b/chicken_wings/data/Chicken_Wings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/Documents/code/chicken_wings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46BDDAD-57FE-EA47-95CB-D041BD81D4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5353DB8F-4B5E-1E40-977F-6F247BCE8E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="34200" windowHeight="21400" activeTab="1" xr2:uid="{29090A6C-1064-F541-B044-7FA7E10DFA86}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="34200" windowHeight="21400" xr2:uid="{29090A6C-1064-F541-B044-7FA7E10DFA86}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1800,7 +1800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{614A498D-8EB1-0644-9825-C15506081E5F}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
@@ -2825,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60157A21-0BBD-8349-8176-E3F8EFEA4634}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>